<commit_message>
update input files for turk tasks
</commit_message>
<xml_diff>
--- a/TurkInputFiles/SpectacularNowFemalePart1.xlsx
+++ b/TurkInputFiles/SpectacularNowFemalePart1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amaye\Desktop\aoibheannamy.github.io\TurkInputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96312246-0411-4FD7-B4D4-5D46AC25688E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D87D53DC-4CAF-4547-934F-B43EA952DCA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="75" yWindow="390" windowWidth="20415" windowHeight="10920" xr2:uid="{F44575C3-1C6A-4706-BE98-C6A195D6AFED}"/>
+    <workbookView xWindow="30" yWindow="0" windowWidth="10440" windowHeight="10920" xr2:uid="{F44575C3-1C6A-4706-BE98-C6A195D6AFED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>image_url</t>
   </si>
@@ -84,18 +84,6 @@
   </si>
   <si>
     <t>https://raw.githubusercontent.com/aoibheannamy/MScProject/master/ImagesForMechTurk/SpectacularNow2.jpg?token=APCQXYU7FERMOZSJWCOQE5S7GQSO20</t>
-  </si>
-  <si>
-    <t>video_url</t>
-  </si>
-  <si>
-    <t>Hit1_video_url_data</t>
-  </si>
-  <si>
-    <t>Hit2_video_url_data</t>
-  </si>
-  <si>
-    <t>Hit3_video_url_data</t>
   </si>
   <si>
     <t>image2_url</t>
@@ -515,204 +503,186 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C48941A9-B169-4429-B4AA-EBAD607E5256}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:XFD20"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>1</v>
       </c>
-      <c r="B17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>2</v>
       </c>
-      <c r="B18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>3</v>
       </c>
-      <c r="B19" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>39</v>
+      <c r="B19" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C5" r:id="rId1" xr:uid="{D674E3B1-2D4C-4E35-B9D6-E4670AFA4D41}"/>
-    <hyperlink ref="C6" r:id="rId2" xr:uid="{10EE8E43-300C-4573-9FB9-8A210EB835F2}"/>
-    <hyperlink ref="C7" r:id="rId3" xr:uid="{00B47EA3-B9A5-4963-9419-E9473B2C929B}"/>
-    <hyperlink ref="C8" r:id="rId4" xr:uid="{1A245FF9-3990-42E3-9D31-87B4FF376C71}"/>
-    <hyperlink ref="C9" r:id="rId5" xr:uid="{15E256FA-8721-4334-89A9-DD37CF8E6AC9}"/>
-    <hyperlink ref="C10" r:id="rId6" xr:uid="{EEB1DF7B-D489-4EB3-8B67-F77F9E0BF92D}"/>
-    <hyperlink ref="C2" r:id="rId7" xr:uid="{6EFBE7FB-5AFA-4517-ABCF-D8B09AE29ED1}"/>
-    <hyperlink ref="C11" r:id="rId8" xr:uid="{33E2386E-8D27-40AB-B450-CFCB053847A1}"/>
-    <hyperlink ref="C12" r:id="rId9" xr:uid="{2D893F0D-D6C6-4494-A15E-B80D3F659A69}"/>
-    <hyperlink ref="C13" r:id="rId10" xr:uid="{4BB8C694-63E7-4129-8E82-D25CE8345FBC}"/>
-    <hyperlink ref="C14" r:id="rId11" xr:uid="{129DC7C0-0DFA-482A-B3A7-75D65D66D7CB}"/>
-    <hyperlink ref="C15" r:id="rId12" xr:uid="{89BCE8AE-3E21-4ED4-B690-29EBD2DFA715}"/>
-    <hyperlink ref="C16" r:id="rId13" xr:uid="{33C585EB-4E80-45CD-A3A5-3189CCAC3AC2}"/>
-    <hyperlink ref="C17" r:id="rId14" xr:uid="{EB835912-CD7C-4B93-A59D-7EFAFCB9BF6D}"/>
-    <hyperlink ref="C18" r:id="rId15" xr:uid="{57A43B54-AC18-4352-ADB9-DC34D2419D84}"/>
-    <hyperlink ref="C19" r:id="rId16" xr:uid="{C885F35C-794E-49D1-B7DD-59D319A09F07}"/>
-    <hyperlink ref="C3" r:id="rId17" xr:uid="{93383A60-266F-4339-B495-1B68837552FC}"/>
-    <hyperlink ref="C4" r:id="rId18" xr:uid="{12F3C139-2666-4298-95A6-8FA541B800CF}"/>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{D674E3B1-2D4C-4E35-B9D6-E4670AFA4D41}"/>
+    <hyperlink ref="B6" r:id="rId2" xr:uid="{10EE8E43-300C-4573-9FB9-8A210EB835F2}"/>
+    <hyperlink ref="B7" r:id="rId3" xr:uid="{00B47EA3-B9A5-4963-9419-E9473B2C929B}"/>
+    <hyperlink ref="B8" r:id="rId4" xr:uid="{1A245FF9-3990-42E3-9D31-87B4FF376C71}"/>
+    <hyperlink ref="B9" r:id="rId5" xr:uid="{15E256FA-8721-4334-89A9-DD37CF8E6AC9}"/>
+    <hyperlink ref="B10" r:id="rId6" xr:uid="{EEB1DF7B-D489-4EB3-8B67-F77F9E0BF92D}"/>
+    <hyperlink ref="B2" r:id="rId7" xr:uid="{6EFBE7FB-5AFA-4517-ABCF-D8B09AE29ED1}"/>
+    <hyperlink ref="B11" r:id="rId8" xr:uid="{33E2386E-8D27-40AB-B450-CFCB053847A1}"/>
+    <hyperlink ref="B12" r:id="rId9" xr:uid="{2D893F0D-D6C6-4494-A15E-B80D3F659A69}"/>
+    <hyperlink ref="B13" r:id="rId10" xr:uid="{4BB8C694-63E7-4129-8E82-D25CE8345FBC}"/>
+    <hyperlink ref="B14" r:id="rId11" xr:uid="{129DC7C0-0DFA-482A-B3A7-75D65D66D7CB}"/>
+    <hyperlink ref="B15" r:id="rId12" xr:uid="{89BCE8AE-3E21-4ED4-B690-29EBD2DFA715}"/>
+    <hyperlink ref="B16" r:id="rId13" xr:uid="{33C585EB-4E80-45CD-A3A5-3189CCAC3AC2}"/>
+    <hyperlink ref="B17" r:id="rId14" xr:uid="{EB835912-CD7C-4B93-A59D-7EFAFCB9BF6D}"/>
+    <hyperlink ref="B18" r:id="rId15" xr:uid="{57A43B54-AC18-4352-ADB9-DC34D2419D84}"/>
+    <hyperlink ref="B19" r:id="rId16" xr:uid="{C885F35C-794E-49D1-B7DD-59D319A09F07}"/>
+    <hyperlink ref="B3" r:id="rId17" xr:uid="{93383A60-266F-4339-B495-1B68837552FC}"/>
+    <hyperlink ref="B4" r:id="rId18" xr:uid="{12F3C139-2666-4298-95A6-8FA541B800CF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>